<commit_message>
Updated Task excel sheet
</commit_message>
<xml_diff>
--- a/Assessment Tasks/Tasks for Code Review 1.xlsx
+++ b/Assessment Tasks/Tasks for Code Review 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Desktop\Edinburgh\Software Engineering Methods\Projects\semAssessment\Assessment Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EE9EB4-6056-4E45-9005-1CEAA298D758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837D1C77-79D9-4AE6-9128-D278E60B4FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Matric</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Tasks defined as user stories</t>
   </si>
   <si>
-    <t>Full use cases defined</t>
-  </si>
-  <si>
     <t>Product Backlog created</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
   </si>
   <si>
     <t>Issues being used on GitHub</t>
-  </si>
-  <si>
-    <t>Use case diagram created</t>
   </si>
   <si>
     <t>Percentage</t>
@@ -217,29 +211,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -263,13 +256,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -311,13 +304,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -862,10 +855,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,7 +871,7 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,141 +881,113 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
         <v>40726424</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="13">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="6" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="6" t="s">
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="14" t="s">
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>40646479</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
-        <v>40646479</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="21">
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="2"/>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>40646484</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="19">
         <v>0.33329999999999999</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="14" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
-        <v>40646484</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="17">
-        <v>0.33329999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="6" t="s">
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="16"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="D12" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>